<commit_message>
Updated test scripts and test data sheet updates
</commit_message>
<xml_diff>
--- a/Test Data/Verify_40V_Calculation_For_FIM.xlsx
+++ b/Test Data/Verify_40V_Calculation_For_FIM.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbhosash\Desktop\31st Jan\NGConsys Automation\Test Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390A8485-2A8C-472D-97FD-A6907B17A2A8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="5604"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Add Panels" sheetId="6" r:id="rId1"/>
@@ -116,9 +117,6 @@
     <t>MX4000</t>
   </si>
   <si>
-    <t>MZX125</t>
-  </si>
-  <si>
     <t>40 V load of XLM 800</t>
   </si>
   <si>
@@ -126,12 +124,15 @@
   </si>
   <si>
     <t>verify40VCalculationforFIM</t>
+  </si>
+  <si>
+    <t>MZX 125</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -280,6 +281,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -294,9 +298,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -577,11 +578,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -595,12 +596,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
       <c r="E1" s="12"/>
       <c r="F1" s="12"/>
       <c r="G1" s="12"/>
@@ -611,12 +612,12 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="16"/>
+      <c r="D2" s="17"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
@@ -627,7 +628,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="8" t="s">
@@ -664,12 +665,12 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
-      <c r="I6" s="17" t="s">
+      <c r="I6" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="20"/>
     </row>
     <row r="7" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
@@ -690,7 +691,7 @@
       <c r="F7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="15" t="s">
         <v>20</v>
       </c>
       <c r="H7" s="14"/>
@@ -704,7 +705,7 @@
         <v>15</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -745,7 +746,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>10</v>

</xml_diff>